<commit_message>
Spelling mistake. added functionality to make save states and reload the data from an external file. refreshed the css and js files
</commit_message>
<xml_diff>
--- a/Data/Scores.xlsx
+++ b/Data/Scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da02ac3bab04d9c0/Documents/Paresley/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="861" documentId="8_{2EAD1506-4EA6-4B40-8F33-8570EE6731CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CE88C19-08F7-4195-9709-AE2FA07C9786}"/>
+  <xr:revisionPtr revIDLastSave="876" documentId="8_{2EAD1506-4EA6-4B40-8F33-8570EE6731CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82550120-E004-4711-A37A-F925A29A894D}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{F197B796-CF8D-4FAA-B522-1A8DE97E8EEA}"/>
+    <workbookView xWindow="5625" yWindow="2535" windowWidth="16875" windowHeight="10522" xr2:uid="{F197B796-CF8D-4FAA-B522-1A8DE97E8EEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Score" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="343">
   <si>
     <t>id</t>
   </si>
@@ -1059,6 +1059,15 @@
   </si>
   <si>
     <t>Baseball bat</t>
+  </si>
+  <si>
+    <t>Flaming Goat</t>
+  </si>
+  <si>
+    <t>Can</t>
+  </si>
+  <si>
+    <t>Make it to the top of the escalator</t>
   </si>
 </sst>
 </file>
@@ -1094,9 +1103,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1411,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA3B05F-F39B-4351-A3D9-B104CE3887D6}">
-  <dimension ref="A1:G179"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView topLeftCell="B106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G119" sqref="G119"/>
+    <sheetView tabSelected="1" topLeftCell="B160" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G183" sqref="G183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5545,6 +5557,29 @@
         <v>304</v>
       </c>
     </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A180" t="s">
+        <v>340</v>
+      </c>
+      <c r="B180">
+        <v>180</v>
+      </c>
+      <c r="C180" t="s">
+        <v>35</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E180">
+        <v>1000</v>
+      </c>
+      <c r="F180">
+        <v>1</v>
+      </c>
+      <c r="G180" t="s">
+        <v>305</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G179" xr:uid="{6BA3B05F-F39B-4351-A3D9-B104CE3887D6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5553,10 +5588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8ADA8F9-7DEF-4981-BAB6-4D3FA5E71785}">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E149" sqref="E2:E149"/>
+    <sheetView topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8407,6 +8442,23 @@
         <v>304</v>
       </c>
     </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A168" t="s">
+        <v>340</v>
+      </c>
+      <c r="B168">
+        <v>166</v>
+      </c>
+      <c r="C168" t="s">
+        <v>341</v>
+      </c>
+      <c r="D168" t="b">
+        <v>0</v>
+      </c>
+      <c r="E168" t="s">
+        <v>305</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E167" xr:uid="{A8ADA8F9-7DEF-4981-BAB6-4D3FA5E71785}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>